<commit_message>
try to get unittest of RecursionError working under "pytest  -s  tests/"
</commit_message>
<xml_diff>
--- a/examples/kinetic_metabolic_model/template.xlsx
+++ b/examples/kinetic_metabolic_model/template.xlsx
@@ -49,10 +49,10 @@
     <t>'!!References'!A1</t>
   </si>
   <si>
-    <t>!!!ObjTables objTablesVersion='1.0.14' date='2020-12-13 14:11:50'</t>
-  </si>
-  <si>
-    <t>!!ObjTables type='TableOfContents' tableFormat='row' description='Table of contents' date='2020-12-13 14:11:50' objTablesVersion='1.0.14'</t>
+    <t>!!!ObjTables objTablesVersion='1.0.14' date='2020-12-13 18:32:51'</t>
+  </si>
+  <si>
+    <t>!!ObjTables type='TableOfContents' tableFormat='row' description='Table of contents' date='2020-12-13 18:32:51' objTablesVersion='1.0.14'</t>
   </si>
   <si>
     <t>!Table</t>
@@ -85,7 +85,7 @@
     <t>References</t>
   </si>
   <si>
-    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-12-13 14:11:50' objTablesVersion='1.0.14'</t>
+    <t>!!ObjTables type='Schema' tableFormat='row' description='Table/model and column/attribute definitions' date='2020-12-13 18:32:51' objTablesVersion='1.0.14'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -451,19 +451,19 @@
     <t>Value</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Compartment' name='Compartments' date='2020-12-13 14:11:50' objTablesVersion='1.0.14'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Compartment' name='Compartments' date='2020-12-13 18:32:51' objTablesVersion='1.0.14'</t>
   </si>
   <si>
     <t>!Id</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Metabolite' name='Metabolites' date='2020-12-13 14:11:50' objTablesVersion='1.0.14'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Metabolite' name='Metabolites' date='2020-12-13 18:32:51' objTablesVersion='1.0.14'</t>
   </si>
   <si>
     <t>!Formula</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Reaction' name='Reactions' date='2020-12-13 14:11:50' objTablesVersion='1.0.14'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Reaction' name='Reactions' date='2020-12-13 18:32:51' objTablesVersion='1.0.14'</t>
   </si>
   <si>
     <t>!Id (iAF1260 [Ref1])</t>
@@ -529,7 +529,7 @@
     <t>!Coupled to biomass</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Regulation' name='Regulations' date='2020-12-13 14:11:50' objTablesVersion='1.0.14'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Regulation' name='Regulations' date='2020-12-13 18:32:51' objTablesVersion='1.0.14'</t>
   </si>
   <si>
     <t>!Reaction</t>
@@ -544,7 +544,7 @@
     <t>!Type [Ref2, Ref3]</t>
   </si>
   <si>
-    <t>!!ObjTables type='Data' tableFormat='row' class='Reference' name='References' date='2020-12-13 14:11:50' objTablesVersion='1.0.14'</t>
+    <t>!!ObjTables type='Data' tableFormat='row' class='Reference' name='References' date='2020-12-13 18:32:51' objTablesVersion='1.0.14'</t>
   </si>
   <si>
     <t>!Title</t>

</xml_diff>